<commit_message>
Added extent reporting logic along with few more cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be19bf08216cfec5/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63FB2909-E92A-4E34-A0B4-6C84E16F017D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{655E224F-5408-4C97-8154-0A9BF51554C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EA3558D3-92A1-4246-8203-194A64704533}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{EA3558D3-92A1-4246-8203-194A64704533}"/>
   </bookViews>
   <sheets>
     <sheet name="ADDTOCART" sheetId="1" r:id="rId1"/>
+    <sheet name="BOOKFLIGHT" sheetId="2" r:id="rId2"/>
+    <sheet name="TESTRUNNER" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>searchtext</t>
   </si>
@@ -57,6 +59,48 @@
   </si>
   <si>
     <t>Macbook</t>
+  </si>
+  <si>
+    <t>departcity</t>
+  </si>
+  <si>
+    <t>arrivalcity</t>
+  </si>
+  <si>
+    <t>Patna</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Lucknow</t>
+  </si>
+  <si>
+    <t>testName</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>bookFlight</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>addToCart</t>
+  </si>
+  <si>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -430,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6866F17E-765E-4A42-B441-6E2D32830AB3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -483,4 +527,94 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A61F45-FA1A-4796-8830-14E70E3E8B05}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DEE95E-0E47-4423-8116-44A9BF824F22}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed dynamic browser implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be19bf08216cfec5/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/BE19BF08216CFEC5/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{655E224F-5408-4C97-8154-0A9BF51554C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A4BC2D3-40FC-43D8-B3FA-49F5EF57BAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{EA3558D3-92A1-4246-8203-194A64704533}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" xr2:uid="{EA3558D3-92A1-4246-8203-194A64704533}"/>
   </bookViews>
   <sheets>
     <sheet name="ADDTOCART" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>searchtext</t>
   </si>
@@ -46,12 +44,18 @@
     <t>execute</t>
   </si>
   <si>
+    <t>browser</t>
+  </si>
+  <si>
     <t>Iphone</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
+    <t>chrome</t>
+  </si>
+  <si>
     <t>TV</t>
   </si>
   <si>
@@ -73,6 +77,9 @@
     <t>Delhi</t>
   </si>
   <si>
+    <t>edge</t>
+  </si>
+  <si>
     <t>Mumbai</t>
   </si>
   <si>
@@ -88,19 +95,10 @@
     <t>testName</t>
   </si>
   <si>
-    <t>browser</t>
-  </si>
-  <si>
     <t>bookFlight</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>addToCart</t>
-  </si>
-  <si>
-    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -472,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6866F17E-765E-4A42-B441-6E2D32830AB3}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -484,44 +482,59 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -531,44 +544,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A61F45-FA1A-4796-8830-14E70E3E8B05}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -580,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DEE95E-0E47-4423-8116-44A9BF824F22}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -592,26 +621,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>